<commit_message>
worked on other endpoints (basics)
</commit_message>
<xml_diff>
--- a/x other/Project Hour Log.xlsx
+++ b/x other/Project Hour Log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\xampp\htdocs\web_backend_test_catering_api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\xampp\htdocs\web_backend_test_catering_api\x other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFCEFCA-69B5-4AAD-B8A3-F4F4949AD91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3EFF3A-4119-450C-AB70-D4291EEA2928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,16 +84,16 @@
     <t>Reading all the information, downloading software and setting up project</t>
   </si>
   <si>
-    <t>Looking inside the repository, routing and trying to understand how all works, playing around a bit.</t>
-  </si>
-  <si>
-    <t>Getting used with the repository</t>
-  </si>
-  <si>
     <t>Setting up database and start working</t>
   </si>
   <si>
-    <t>Createad the database and populated, start working on /getall and /getone</t>
+    <t>Research and preparation</t>
+  </si>
+  <si>
+    <t>Looking through the repository, routing and trying to understand how it all works, playing around a bit.</t>
+  </si>
+  <si>
+    <t>Createad and populated the database, start working on /getall and /getone endpoints</t>
   </si>
 </sst>
 </file>
@@ -353,14 +353,14 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -797,7 +797,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -809,22 +809,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -854,7 +854,7 @@
       <c r="C4" s="7">
         <v>45062</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="8"/>
@@ -870,49 +870,53 @@
       <c r="C5" s="7">
         <v>45063</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>9</v>
+      <c r="D5" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
       </c>
       <c r="C6" s="7">
-        <v>45064</v>
-      </c>
-      <c r="D6" s="20" t="s">
+        <v>45063</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="20"/>
+      <c r="C7" s="7">
+        <v>45064</v>
+      </c>
+      <c r="D7" s="18"/>
       <c r="E7" s="8"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="20"/>
+      <c r="C8" s="7">
+        <v>45064</v>
+      </c>
+      <c r="D8" s="18"/>
       <c r="E8" s="8"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="20"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="8"/>
       <c r="F9" s="4"/>
     </row>
@@ -920,7 +924,7 @@
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="20"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="8"/>
       <c r="F10" s="4"/>
     </row>
@@ -928,7 +932,7 @@
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="20"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="8"/>
       <c r="F11" s="4"/>
     </row>
@@ -936,7 +940,7 @@
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="20"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="8"/>
       <c r="F12" s="4"/>
     </row>
@@ -944,7 +948,7 @@
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="20"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="8"/>
       <c r="F13" s="4"/>
     </row>
@@ -952,7 +956,7 @@
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="20"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="8"/>
       <c r="F14" s="4"/>
     </row>
@@ -960,7 +964,7 @@
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="20"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="8"/>
       <c r="F15" s="4"/>
     </row>
@@ -968,7 +972,7 @@
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="20"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="8"/>
       <c r="F16" s="4"/>
     </row>
@@ -976,7 +980,7 @@
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="20"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="8"/>
       <c r="F17" s="4"/>
     </row>
@@ -984,7 +988,7 @@
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="20"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="8"/>
       <c r="F18" s="4"/>
     </row>
@@ -992,7 +996,7 @@
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="20"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="8"/>
       <c r="F19" s="4"/>
     </row>
@@ -1000,7 +1004,7 @@
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="20"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="8"/>
       <c r="F20" s="4"/>
     </row>
@@ -1008,7 +1012,7 @@
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="20"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="8"/>
       <c r="F21" s="4"/>
     </row>
@@ -1016,7 +1020,7 @@
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="20"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="8"/>
       <c r="F22" s="4"/>
     </row>
@@ -1024,7 +1028,7 @@
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="20"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="8"/>
       <c r="F23" s="4"/>
     </row>
@@ -1032,7 +1036,7 @@
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="20"/>
+      <c r="D24" s="18"/>
       <c r="E24" s="8"/>
       <c r="F24" s="4"/>
     </row>
@@ -1040,7 +1044,7 @@
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="20"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="8"/>
       <c r="F25" s="4"/>
     </row>
@@ -1048,7 +1052,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="20"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="8"/>
       <c r="F26" s="4"/>
     </row>
@@ -1056,7 +1060,7 @@
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="20"/>
+      <c r="D27" s="18"/>
       <c r="E27" s="8"/>
       <c r="F27" s="4"/>
     </row>
@@ -1064,7 +1068,7 @@
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="20"/>
+      <c r="D28" s="18"/>
       <c r="E28" s="8"/>
       <c r="F28" s="4"/>
     </row>
@@ -1076,7 +1080,7 @@
       <c r="E29" s="11"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
pagination, sanitation, request body format
</commit_message>
<xml_diff>
--- a/x other/Project Hour Log.xlsx
+++ b/x other/Project Hour Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\xampp\htdocs\web_backend_test_catering_api\x other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5E0EAB-D490-4E95-B0AE-1AA2B62D8D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA74FB8-EE17-4843-A0E5-C1BB255ADA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <r>
       <rPr>
@@ -78,28 +78,34 @@
     <t>Total amount of hours</t>
   </si>
   <si>
-    <t>Project set up</t>
-  </si>
-  <si>
-    <t>Reading all the information, downloading software and setting up project</t>
-  </si>
-  <si>
     <t>Setting up database and start working</t>
   </si>
   <si>
     <t>Research and preparation</t>
   </si>
   <si>
-    <t>Looking through the repository, routing and trying to understand how it all works, playing around a bit.</t>
-  </si>
-  <si>
-    <t>Createad and populated the database, start working on /getall and /getone endpoints</t>
-  </si>
-  <si>
     <t>Working on requirements</t>
   </si>
   <si>
-    <t xml:space="preserve">Created all endpoints on a basic level and tested them. </t>
+    <t>Getting to know the project</t>
+  </si>
+  <si>
+    <t>Reading all the information a few times, downloading and installing software and setting up project. I had some problems with installing the composer and routing.</t>
+  </si>
+  <si>
+    <t>Createad and populated the database, start working on /getall and /getone endpoints. At first I created a repository class (I am used to MVC) in where I was having the queries, but because of a db problem I moved it all in controller.</t>
+  </si>
+  <si>
+    <t>Working on assignment</t>
+  </si>
+  <si>
+    <t>Created all endpoints on a basic level and tested them.  I created a new method that is pretty much same as executeQuery but it returns an array instead of boolean. For testing purposes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking through the repository, routing and trying to understand how it all works. Since I didn't develop REST API in PHP before I was a bit confused, watched a short tutorial on youtube (https://www.youtube.com/watch?v=pqEONSbXeSQ) and then started to play around. </t>
+  </si>
+  <si>
+    <t>Going over the requirements and improving endpoints according to REST style. Made a new method to get the request data based on content type and sanitize it. Implemented pagination.</t>
   </si>
 </sst>
 </file>
@@ -803,7 +809,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -850,25 +856,25 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="7">
         <v>45062</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="6">
         <v>2</v>
@@ -877,14 +883,14 @@
         <v>45063</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
@@ -898,7 +904,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -914,13 +920,19 @@
       <c r="E7" s="8"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
+    <row r="8" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6">
+        <v>2</v>
+      </c>
       <c r="C8" s="7">
-        <v>45064</v>
-      </c>
-      <c r="D8" s="18"/>
+        <v>45065</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="4"/>
     </row>
@@ -1098,7 +1110,7 @@
       </c>
       <c r="B30" s="13">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>

</xml_diff>

<commit_message>
updated PUT and POST endpoints
</commit_message>
<xml_diff>
--- a/x other/Project Hour Log.xlsx
+++ b/x other/Project Hour Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\xampp\htdocs\web_backend_test_catering_api\x other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7320019B-5F81-4DF4-B833-2C6B1122E06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED43E43-7F74-45AA-9593-4F065323440C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <r>
       <rPr>
@@ -114,10 +114,16 @@
     <t>While working on user story 3, I realised that I missed something in the requirements regarding the database (a Facility can have multiple Tags), so I had to change the database and all the previous queries. After that implemented the search endpoint successfully. Here I understood that I need extra methods for creating and updating a new tag/location (so when creating a new facility, you can create a new location or tag instead of choosing from existing ones),</t>
   </si>
   <si>
-    <t xml:space="preserve">Fix POST and PUT </t>
-  </si>
-  <si>
-    <t>Changed the createOne and updateOne (facility) methods in order to be able to add or update a location or tag.</t>
+    <t>Created a method to manage locations and added it inside createOne and updateOne method, so when a new facility is created or updated - a new location will be inserted in database if it's not there already.</t>
+  </si>
+  <si>
+    <t>Manage Locations</t>
+  </si>
+  <si>
+    <t>Manage Tags</t>
+  </si>
+  <si>
+    <t>Here I had some problems with the tags. Since I added a new table in database (facility_tags) everything changed and got a bit more complicated. Then I took it step by step and made a lot of methods for it. In the end I still have a problem when inserting a new facility with tags, but i managed to fix the update method completly.</t>
   </si>
 </sst>
 </file>
@@ -820,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -884,7 +890,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -948,7 +954,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -964,9 +970,9 @@
       <c r="E9" s="8"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="6">
         <v>1</v>
@@ -975,16 +981,24 @@
         <v>45066</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="18"/>
+    <row r="11" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7">
+        <v>45066</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>22</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="4"/>
     </row>
@@ -1138,7 +1152,7 @@
       </c>
       <c r="B30" s="13">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>

</xml_diff>

<commit_message>
fixed sanitizing, search filter, pagination
</commit_message>
<xml_diff>
--- a/x other/Project Hour Log.xlsx
+++ b/x other/Project Hour Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\xampp\htdocs\web_backend_test_catering_api\x other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2CBA45-D2FB-470E-9784-65CBEEC09AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0298CB59-A6FF-4CBF-85BF-D4532B3B551F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <r>
       <rPr>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Checking everything again, here I found some problems that could be improved, but I don't have more time right now. It was a new experience working with API in PHP and I'd like to learn more about it.</t>
+  </si>
+  <si>
+    <t>Applying feedback</t>
+  </si>
+  <si>
+    <t>Fixed search endpoint to apply none,1 or more filters. Returning the facility when creating and updating it.Removed some unnecessary comments, fixed pagination, added sanitization to all other endpoints, added model classes.</t>
   </si>
 </sst>
 </file>
@@ -844,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1036,7 +1042,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
@@ -1052,7 +1058,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1076,15 +1082,23 @@
       <c r="E15" s="8"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="18"/>
+    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7">
+        <v>45085</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1194,7 +1208,7 @@
       </c>
       <c r="B30" s="13">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>

</xml_diff>